<commit_message>
LotteryTrackerFile test file updated
</commit_message>
<xml_diff>
--- a/LotteryTrackerTests/TestFiles/LotteryTrackerFile.xlsx
+++ b/LotteryTrackerTests/TestFiles/LotteryTrackerFile.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7398" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7396" uniqueCount="134">
   <si>
     <t>Dias</t>
   </si>
@@ -437,7 +437,7 @@
     <numFmt numFmtId="166" formatCode="&quot;$&quot;\ #,##0.00"/>
     <numFmt numFmtId="167" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -564,8 +564,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -677,18 +685,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF6600"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0000FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF948A54"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1061,7 +1057,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="255">
+  <cellXfs count="254">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1732,9 +1728,7 @@
     <xf numFmtId="0" fontId="16" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1789,6 +1783,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2041,23 +2036,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="97066368"/>
-        <c:axId val="97076352"/>
+        <c:axId val="94563328"/>
+        <c:axId val="94442240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97066368"/>
+        <c:axId val="94563328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97076352"/>
+        <c:crossAx val="94442240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97076352"/>
+        <c:axId val="94442240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2065,7 +2060,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0_ ;\-#,##0\ " sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97066368"/>
+        <c:crossAx val="94563328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2077,7 +2072,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000389" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000389" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000455" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000455" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2426,36 +2421,36 @@
   <sheetData>
     <row r="1" spans="1:27" s="61" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="60"/>
-      <c r="B1" s="247" t="s">
+      <c r="B1" s="245" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="247"/>
-      <c r="D1" s="247"/>
-      <c r="E1" s="248"/>
-      <c r="F1" s="241" t="s">
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="239" t="s">
         <v>99</v>
       </c>
-      <c r="G1" s="241"/>
-      <c r="H1" s="241"/>
-      <c r="I1" s="242"/>
-      <c r="J1" s="243" t="s">
+      <c r="G1" s="239"/>
+      <c r="H1" s="239"/>
+      <c r="I1" s="240"/>
+      <c r="J1" s="241" t="s">
         <v>104</v>
       </c>
-      <c r="K1" s="243"/>
-      <c r="L1" s="243"/>
-      <c r="M1" s="244"/>
-      <c r="N1" s="245" t="s">
+      <c r="K1" s="241"/>
+      <c r="L1" s="241"/>
+      <c r="M1" s="242"/>
+      <c r="N1" s="243" t="s">
         <v>105</v>
       </c>
-      <c r="O1" s="245"/>
-      <c r="P1" s="245"/>
-      <c r="Q1" s="246"/>
-      <c r="R1" s="239" t="s">
+      <c r="O1" s="243"/>
+      <c r="P1" s="243"/>
+      <c r="Q1" s="244"/>
+      <c r="R1" s="237" t="s">
         <v>107</v>
       </c>
-      <c r="S1" s="239"/>
-      <c r="T1" s="239"/>
-      <c r="U1" s="240"/>
+      <c r="S1" s="237"/>
+      <c r="T1" s="237"/>
+      <c r="U1" s="238"/>
       <c r="X1" s="71"/>
       <c r="Y1" s="71"/>
       <c r="Z1" s="71"/>
@@ -5597,10 +5592,10 @@
     </row>
     <row r="43" spans="1:27" ht="15.75">
       <c r="A43" s="56"/>
-      <c r="B43" s="237"/>
-      <c r="C43" s="238"/>
-      <c r="D43" s="238"/>
-      <c r="E43" s="238"/>
+      <c r="B43" s="235"/>
+      <c r="C43" s="236"/>
+      <c r="D43" s="236"/>
+      <c r="E43" s="236"/>
       <c r="F43" s="55"/>
     </row>
     <row r="44" spans="1:27" ht="15.75">
@@ -8749,12 +8744,12 @@
       <c r="M79" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="O79" s="249" t="s">
+      <c r="O79" s="247" t="s">
         <v>95</v>
       </c>
-      <c r="P79" s="250"/>
-      <c r="Q79" s="250"/>
-      <c r="R79" s="251"/>
+      <c r="P79" s="248"/>
+      <c r="Q79" s="248"/>
+      <c r="R79" s="249"/>
     </row>
     <row r="80" spans="1:18" ht="15.75" thickBot="1">
       <c r="A80" s="130">
@@ -11039,11 +11034,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V108"/>
+  <dimension ref="A1:V106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A255" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A104" sqref="A104:XFD267"/>
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -12527,12 +12522,12 @@
         <v>18</v>
       </c>
       <c r="N34" s="127"/>
-      <c r="O34" s="249" t="s">
+      <c r="O34" s="247" t="s">
         <v>95</v>
       </c>
-      <c r="P34" s="250"/>
-      <c r="Q34" s="250"/>
-      <c r="R34" s="251"/>
+      <c r="P34" s="248"/>
+      <c r="Q34" s="248"/>
+      <c r="R34" s="249"/>
       <c r="S34" s="127"/>
       <c r="T34" s="127"/>
       <c r="U34" s="127"/>
@@ -15847,13 +15842,13 @@
         <v>30</v>
       </c>
       <c r="F103" s="11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G103" s="10" t="s">
         <v>23</v>
       </c>
       <c r="H103" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I103" s="20" t="s">
         <v>71</v>
@@ -15881,99 +15876,26 @@
       <c r="V103" s="127"/>
     </row>
     <row r="104" spans="1:22">
-      <c r="A104" s="234">
+      <c r="A104" s="69">
         <v>12</v>
       </c>
-      <c r="B104" s="234" t="s">
+      <c r="B104" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="C104" s="234"/>
-      <c r="D104" s="234"/>
-      <c r="E104" s="234"/>
-      <c r="F104" s="234"/>
-      <c r="G104" s="234"/>
-      <c r="H104" s="234"/>
-      <c r="I104" s="234"/>
-      <c r="J104" s="234"/>
-      <c r="K104" s="234"/>
-      <c r="L104" s="234"/>
-      <c r="M104" s="234"/>
     </row>
     <row r="105" spans="1:22">
-      <c r="A105" s="234">
+      <c r="B105" s="234"/>
+    </row>
+    <row r="106" spans="1:22">
+      <c r="A106" s="69">
         <v>12</v>
       </c>
-      <c r="B105" s="234" t="s">
+      <c r="B106" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="C105" s="234"/>
-      <c r="D105" s="234"/>
-      <c r="E105" s="234"/>
-      <c r="F105" s="234"/>
-      <c r="G105" s="234"/>
-      <c r="H105" s="234"/>
-      <c r="I105" s="234"/>
-      <c r="J105" s="234"/>
-      <c r="K105" s="234"/>
-      <c r="L105" s="234"/>
-      <c r="M105" s="234"/>
-    </row>
-    <row r="106" spans="1:22">
-      <c r="A106" s="235">
-        <v>12</v>
-      </c>
-      <c r="B106" s="235" t="s">
-        <v>9</v>
-      </c>
-      <c r="C106" s="235"/>
-      <c r="D106" s="235"/>
-      <c r="E106" s="235"/>
-      <c r="F106" s="235"/>
-      <c r="G106" s="235"/>
-      <c r="H106" s="235"/>
-      <c r="I106" s="235"/>
-      <c r="J106" s="235"/>
-      <c r="K106" s="235"/>
-      <c r="L106" s="235"/>
-      <c r="M106" s="235"/>
-    </row>
-    <row r="107" spans="1:22">
-      <c r="A107" s="236">
-        <v>12</v>
-      </c>
-      <c r="B107" s="236" t="s">
-        <v>9</v>
-      </c>
-      <c r="C107" s="236"/>
-      <c r="D107" s="236"/>
-      <c r="E107" s="236"/>
-      <c r="F107" s="236"/>
-      <c r="G107" s="236"/>
-      <c r="H107" s="236"/>
-      <c r="I107" s="236"/>
-      <c r="J107" s="236"/>
-      <c r="K107" s="236"/>
-      <c r="L107" s="236"/>
-      <c r="M107" s="236"/>
-    </row>
-    <row r="108" spans="1:22">
-      <c r="A108" s="236">
-        <v>12</v>
-      </c>
-      <c r="B108" s="236" t="s">
-        <v>9</v>
-      </c>
-      <c r="C108" s="236"/>
-      <c r="D108" s="236"/>
-      <c r="E108" s="236"/>
-      <c r="F108" s="236"/>
-      <c r="G108" s="236"/>
-      <c r="H108" s="236"/>
-      <c r="I108" s="236"/>
-      <c r="J108" s="236"/>
-      <c r="K108" s="236"/>
-      <c r="L108" s="236"/>
-      <c r="M108" s="236"/>
+      <c r="I106" s="253" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -16014,23 +15936,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A1" s="252" t="s">
+      <c r="A1" s="250" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="253"/>
-      <c r="C1" s="253"/>
-      <c r="D1" s="254" t="s">
+      <c r="B1" s="251"/>
+      <c r="C1" s="251"/>
+      <c r="D1" s="252" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="250"/>
-      <c r="I1" s="250"/>
-      <c r="J1" s="250"/>
-      <c r="K1" s="250"/>
-      <c r="L1" s="250"/>
-      <c r="M1" s="251"/>
+      <c r="E1" s="248"/>
+      <c r="F1" s="248"/>
+      <c r="G1" s="248"/>
+      <c r="H1" s="248"/>
+      <c r="I1" s="248"/>
+      <c r="J1" s="248"/>
+      <c r="K1" s="248"/>
+      <c r="L1" s="248"/>
+      <c r="M1" s="249"/>
     </row>
     <row r="2" spans="1:14" ht="13.5" thickBot="1">
       <c r="A2" s="125" t="s">
@@ -17206,12 +17128,12 @@
       <c r="M35" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="O35" s="249" t="s">
+      <c r="O35" s="247" t="s">
         <v>95</v>
       </c>
-      <c r="P35" s="250"/>
-      <c r="Q35" s="250"/>
-      <c r="R35" s="251"/>
+      <c r="P35" s="248"/>
+      <c r="Q35" s="248"/>
+      <c r="R35" s="249"/>
     </row>
     <row r="36" spans="1:18" ht="13.5" thickBot="1">
       <c r="A36" s="131">
@@ -20388,23 +20310,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.5" thickBot="1">
-      <c r="A1" s="252" t="s">
+      <c r="A1" s="250" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="253"/>
-      <c r="C1" s="253"/>
-      <c r="D1" s="254" t="s">
+      <c r="B1" s="251"/>
+      <c r="C1" s="251"/>
+      <c r="D1" s="252" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="250"/>
-      <c r="I1" s="250"/>
-      <c r="J1" s="250"/>
-      <c r="K1" s="250"/>
-      <c r="L1" s="250"/>
-      <c r="M1" s="251"/>
+      <c r="E1" s="248"/>
+      <c r="F1" s="248"/>
+      <c r="G1" s="248"/>
+      <c r="H1" s="248"/>
+      <c r="I1" s="248"/>
+      <c r="J1" s="248"/>
+      <c r="K1" s="248"/>
+      <c r="L1" s="248"/>
+      <c r="M1" s="249"/>
     </row>
     <row r="2" spans="1:13" ht="13.5" thickBot="1">
       <c r="A2" s="125" t="s">
@@ -21422,12 +21344,12 @@
       <c r="M35" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="O35" s="249" t="s">
+      <c r="O35" s="247" t="s">
         <v>95</v>
       </c>
-      <c r="P35" s="250"/>
-      <c r="Q35" s="250"/>
-      <c r="R35" s="251"/>
+      <c r="P35" s="248"/>
+      <c r="Q35" s="248"/>
+      <c r="R35" s="249"/>
     </row>
     <row r="36" spans="1:18" ht="13.5" thickBot="1">
       <c r="A36" s="131">
@@ -24500,23 +24422,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.5" thickBot="1">
-      <c r="A1" s="252" t="s">
+      <c r="A1" s="250" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="253"/>
-      <c r="C1" s="253"/>
-      <c r="D1" s="254" t="s">
+      <c r="B1" s="251"/>
+      <c r="C1" s="251"/>
+      <c r="D1" s="252" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="250"/>
-      <c r="I1" s="250"/>
-      <c r="J1" s="250"/>
-      <c r="K1" s="250"/>
-      <c r="L1" s="250"/>
-      <c r="M1" s="251"/>
+      <c r="E1" s="248"/>
+      <c r="F1" s="248"/>
+      <c r="G1" s="248"/>
+      <c r="H1" s="248"/>
+      <c r="I1" s="248"/>
+      <c r="J1" s="248"/>
+      <c r="K1" s="248"/>
+      <c r="L1" s="248"/>
+      <c r="M1" s="249"/>
     </row>
     <row r="2" spans="1:13" ht="13.5" thickBot="1">
       <c r="A2" s="125" t="s">
@@ -25702,12 +25624,12 @@
       <c r="M35" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="O35" s="249" t="s">
+      <c r="O35" s="247" t="s">
         <v>95</v>
       </c>
-      <c r="P35" s="250"/>
-      <c r="Q35" s="250"/>
-      <c r="R35" s="251"/>
+      <c r="P35" s="248"/>
+      <c r="Q35" s="248"/>
+      <c r="R35" s="249"/>
     </row>
     <row r="36" spans="1:18" ht="13.5" thickBot="1">
       <c r="A36" s="131">
@@ -31795,12 +31717,12 @@
       <c r="M82" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="O82" s="249" t="s">
+      <c r="O82" s="247" t="s">
         <v>95</v>
       </c>
-      <c r="P82" s="250"/>
-      <c r="Q82" s="250"/>
-      <c r="R82" s="251"/>
+      <c r="P82" s="248"/>
+      <c r="Q82" s="248"/>
+      <c r="R82" s="249"/>
     </row>
     <row r="83" spans="1:18" ht="15.75" thickBot="1">
       <c r="A83" s="130">
@@ -36181,12 +36103,12 @@
       <c r="K84" s="44"/>
       <c r="L84" s="44"/>
       <c r="M84" s="45"/>
-      <c r="O84" s="249" t="s">
+      <c r="O84" s="247" t="s">
         <v>95</v>
       </c>
-      <c r="P84" s="250"/>
-      <c r="Q84" s="250"/>
-      <c r="R84" s="251"/>
+      <c r="P84" s="248"/>
+      <c r="Q84" s="248"/>
+      <c r="R84" s="249"/>
     </row>
     <row r="85" spans="1:18" ht="15.75" thickBot="1">
       <c r="A85" s="130">
@@ -40489,12 +40411,12 @@
       <c r="K84" s="44"/>
       <c r="L84" s="44"/>
       <c r="M84" s="45"/>
-      <c r="O84" s="249" t="s">
+      <c r="O84" s="247" t="s">
         <v>95</v>
       </c>
-      <c r="P84" s="250"/>
-      <c r="Q84" s="250"/>
-      <c r="R84" s="251"/>
+      <c r="P84" s="248"/>
+      <c r="Q84" s="248"/>
+      <c r="R84" s="249"/>
     </row>
     <row r="85" spans="1:18" ht="15.75" thickBot="1">
       <c r="A85" s="130">

</xml_diff>